<commit_message>
updated 2013pnas paper citation
</commit_message>
<xml_diff>
--- a/cv.xlsx
+++ b/cv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/git/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE3ED89-7E1E-B746-9ED9-38EDA3561987}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0EFE42-BD4D-5C4D-AAED-B564D9CCC974}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="4560" windowWidth="28160" windowHeight="16440" activeTab="1" xr2:uid="{49BEF855-14FC-304C-9B93-8FA563204E38}"/>
+    <workbookView xWindow="5440" yWindow="4560" windowWidth="28160" windowHeight="16440" xr2:uid="{49BEF855-14FC-304C-9B93-8FA563204E38}"/>
   </bookViews>
   <sheets>
     <sheet name="positions" sheetId="1" r:id="rId1"/>
@@ -988,9 +988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3854BA9-2B2F-4849-8499-B1FE2AB1C1F4}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1878,22 +1878,22 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="G28">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="I28" t="s">
         <v>10</v>
@@ -1910,28 +1910,28 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
       </c>
       <c r="F29">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G29">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="H29" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="I29" t="s">
         <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1942,10 +1942,10 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1957,13 +1957,13 @@
         <v>2011</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="I30" t="s">
         <v>10</v>
       </c>
       <c r="J30" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2339,9 +2339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D4E204-A097-E246-8420-89EA1CD35275}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3226,22 +3226,22 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="G28">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="I28" t="s">
         <v>10</v>
@@ -3258,28 +3258,28 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
       </c>
       <c r="F29">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G29">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="H29" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="I29" t="s">
         <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -3290,10 +3290,10 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -3305,13 +3305,13 @@
         <v>2011</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="I30" t="s">
         <v>10</v>
       </c>
       <c r="J30" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>